<commit_message>
Final draft for thesis
</commit_message>
<xml_diff>
--- a/Overlaps/GO/genes.xlsx
+++ b/Overlaps/GO/genes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1180" windowWidth="24460" windowHeight="14820" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="15340" yWindow="460" windowWidth="10000" windowHeight="13040" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>malvolio (mvl)</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>Gene or process</t>
+  </si>
+  <si>
+    <t>peptidoglycan recognition proteins</t>
   </si>
 </sst>
 </file>
@@ -479,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A42"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,82 +573,85 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="30" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:1" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>11</v>
       </c>
@@ -677,26 +683,21 @@
     </row>
     <row r="38" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>